<commit_message>
Selectors css box model
</commit_message>
<xml_diff>
--- a/Omnifood/Documantation/omniFood.xlsx
+++ b/Omnifood/Documantation/omniFood.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="2655" windowHeight="3240" tabRatio="826"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="2655" windowHeight="3240" tabRatio="826" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Duration Meter" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="285">
   <si>
     <t>Day</t>
   </si>
@@ -1262,9 +1262,6 @@
   </si>
   <si>
     <t>human - &gt; characteristics</t>
-  </si>
-  <si>
-    <t>HTML - Cascading Style Sheets</t>
   </si>
   <si>
     <t>Content</t>
@@ -1655,12 +1652,296 @@
   <si>
     <t>27/1/18</t>
   </si>
+  <si>
+    <t>Commits</t>
+  </si>
+  <si>
+    <t>git log origin/master..HEAD</t>
+  </si>
+  <si>
+    <t>view the local commits made</t>
+  </si>
+  <si>
+    <t>git diff origin/master..HEAD</t>
+  </si>
+  <si>
+    <t>view the difference between local and remote</t>
+  </si>
+  <si>
+    <r>
+      <t>margin-left</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>auto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>margin-right</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>auto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1140px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>context element</t>
+  </si>
+  <si>
+    <t>(browser,screen..)</t>
+  </si>
+  <si>
+    <t>adjusted automatically according to the container width from the left &amp; the context element</t>
+  </si>
+  <si>
+    <t>adjusted automatically according to the container width from the right &amp; the context element</t>
+  </si>
+  <si>
+    <t>floatL: left/right;</t>
+  </si>
+  <si>
+    <t>Make an element float in the assigned location</t>
+  </si>
+  <si>
+    <r>
+      <t>clear</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> both</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>Do not allow floating elements on the left or the right side of a specified element
+can be a &lt;div&gt; &lt;p&gt; …</t>
+  </si>
+  <si>
+    <r>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> none</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;
+display: inline;
+display: block;
+display: inline-block;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The display property specifies the display behavior of an element.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Every element on a web page is a rectangular box. The CSS display property determines how that rectangular box behaves.</t>
+    </r>
+  </si>
+  <si>
+    <t>a:after {
+    content: "(" attr(href) ")";
+}</t>
+  </si>
+  <si>
+    <t>The content property is used to insert generated content.
+Will display the href attribute of every thing after the context of a href.
+Or for that matter every content after every element.</t>
+  </si>
+  <si>
+    <t>Margin Box</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Top -&gt; right -&gt; bottom -&gt; left</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>Order Clock wise</t>
+  </si>
+  <si>
+    <t>margin: top right bottom left</t>
+  </si>
+  <si>
+    <t>border &lt;width size&gt; &lt;type&gt; &lt;color&gt;
+size : px
+type : solid
+color: #000000-#ffffff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set the border </t>
+  </si>
+  <si>
+    <t>CSS Selectors LINK</t>
+  </si>
+  <si>
+    <t>CSS - Cascading Style Sheets</t>
+  </si>
+  <si>
+    <t>CSS Selectors can select all / part of the selection</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="55" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1994,8 +2275,57 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000CD"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2056,8 +2386,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2080,13 +2428,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2261,9 +2635,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="33" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2321,8 +2692,48 @@
     <xf numFmtId="0" fontId="43" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2451,7 +2862,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2537,11 +2947,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="80602624"/>
-        <c:axId val="68579264"/>
+        <c:axId val="97117696"/>
+        <c:axId val="53768128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80602624"/>
+        <c:axId val="97117696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2579,7 +2989,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68579264"/>
+        <c:crossAx val="53768128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2587,7 +2997,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68579264"/>
+        <c:axId val="53768128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2635,7 +3045,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80602624"/>
+        <c:crossAx val="97117696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2650,7 +3060,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2722,7 +3131,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2795,7 +3203,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2970,11 +3377,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="68580992"/>
-        <c:axId val="68581568"/>
+        <c:axId val="53769856"/>
+        <c:axId val="53770432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68580992"/>
+        <c:axId val="53769856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3012,12 +3419,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68581568"/>
+        <c:crossAx val="53770432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68581568"/>
+        <c:axId val="53770432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3065,7 +3472,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68580992"/>
+        <c:crossAx val="53769856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3954,15 +4361,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:colOff>781050</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3986,7 +4393,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7953375" y="1162050"/>
+          <a:off x="10944225" y="1209675"/>
           <a:ext cx="6105525" cy="1962150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4008,16 +4415,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>3343275</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>3352800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4041,7 +4448,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7962900" y="3667125"/>
+          <a:off x="11820525" y="2905125"/>
           <a:ext cx="3352800" cy="4667250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6033,7 +6440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -6104,13 +6511,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>249</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>194</v>
       </c>
       <c r="E3" s="10">
         <f>VALUE(LEFT(D3,2))*60+VALUE(RIGHT(D3,2))</f>
@@ -6145,13 +6552,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E4" s="10">
         <f>VALUE(LEFT(D4,2))*60+VALUE(RIGHT(D4,2))</f>
@@ -6185,13 +6592,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5" s="60">
         <v>43283</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E5" s="10">
         <f>VALUE(LEFT(D5,2))*60+VALUE(RIGHT(D5,2))</f>
@@ -7170,145 +7577,270 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="84.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
+      <c r="A1" s="92" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
       <c r="G1" s="59" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G2" s="65" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G2" s="65" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="94" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="95" t="s">
+        <v>282</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="G3" s="66" t="s">
+        <v>217</v>
+      </c>
+      <c r="H3" s="67" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="G3" s="67" t="s">
+      <c r="I3" s="67" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="105" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="105" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="G4" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="H3" s="68" t="s">
-        <v>215</v>
-      </c>
-      <c r="I3" s="68" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="H4" s="69" t="s">
-        <v>217</v>
+      <c r="H4" s="68" t="s">
+        <v>216</v>
       </c>
       <c r="I4" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="59" t="s">
-        <v>222</v>
-      </c>
-      <c r="G5" s="70" t="s">
-        <v>220</v>
-      </c>
-      <c r="H5" s="71" t="s">
-        <v>216</v>
+      <c r="B5" s="96" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="70"/>
+      <c r="G5" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="H5" s="70" t="s">
+        <v>215</v>
       </c>
       <c r="I5" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="70" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="70" t="s">
         <v>208</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C7" s="68" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>209</v>
-      </c>
-      <c r="C7" s="66" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="70" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="70" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="96" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>223</v>
-      </c>
-      <c r="C8" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="59" t="s">
+      <c r="C9" s="70"/>
+      <c r="D9" s="93" t="s">
+        <v>278</v>
+      </c>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="70" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C10" s="70" t="s">
+        <v>279</v>
+      </c>
+      <c r="D10" s="93" t="s">
+        <v>275</v>
+      </c>
+      <c r="E10" s="93"/>
+      <c r="F10" s="93"/>
+    </row>
+    <row r="11" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="70" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="70" t="s">
         <v>228</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" s="91" t="s">
+        <v>276</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="F11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="70"/>
+      <c r="C12" s="70" t="s">
+        <v>257</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="97" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" s="104" t="s">
+        <v>260</v>
+      </c>
+      <c r="C13" s="70" t="s">
+        <v>255</v>
+      </c>
+      <c r="D13" s="91" t="s">
+        <v>277</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="F13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="70" t="s">
+        <v>259</v>
+      </c>
+      <c r="B14" s="104" t="s">
+        <v>261</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="70" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C15" s="70" t="s">
         <v>230</v>
       </c>
-      <c r="C11" t="s">
-        <v>231</v>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="70" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" s="70" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="98" t="s">
+        <v>265</v>
+      </c>
+      <c r="C17" s="70" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B18" s="99" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="100" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B19" s="101" t="s">
+        <v>269</v>
+      </c>
+      <c r="C19" s="70" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B20" s="102" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" s="103" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -7322,18 +7854,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="75"/>
-    <col min="2" max="2" width="84.5703125" style="75" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" style="75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="75"/>
-    <col min="5" max="5" width="18.5703125" style="75" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="75"/>
-    <col min="8" max="8" width="23" style="75"/>
-    <col min="9" max="9" width="22.5703125" style="75" customWidth="1"/>
-    <col min="10" max="10" width="64" style="75"/>
-    <col min="11" max="11" width="17.7109375" style="75"/>
-    <col min="12" max="1025" width="8.5703125" style="75"/>
+    <col min="1" max="1" width="28.85546875" style="74"/>
+    <col min="2" max="2" width="84.5703125" style="74" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="74"/>
+    <col min="5" max="5" width="18.5703125" style="74" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="74" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="74"/>
+    <col min="8" max="8" width="23" style="74"/>
+    <col min="9" max="9" width="22.5703125" style="74" customWidth="1"/>
+    <col min="10" max="10" width="64" style="74"/>
+    <col min="11" max="11" width="17.7109375" style="74"/>
+    <col min="12" max="1025" width="8.5703125" style="74"/>
     <col min="1026" max="16384" width="9.140625" style="61"/>
   </cols>
   <sheetData>
@@ -7342,13 +7874,13 @@
       <c r="B1" s="61"/>
       <c r="C1" s="64"/>
       <c r="D1" s="64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E1" s="64"/>
       <c r="F1" s="64"/>
       <c r="G1" s="61"/>
-      <c r="H1" s="72" t="s">
-        <v>233</v>
+      <c r="H1" s="71" t="s">
+        <v>232</v>
       </c>
       <c r="I1" s="61"/>
       <c r="J1" s="61"/>
@@ -7358,7 +7890,7 @@
       <c r="A2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="71" t="s">
         <v>156</v>
       </c>
       <c r="C2" s="3"/>
@@ -7368,25 +7900,25 @@
         <v>189</v>
       </c>
       <c r="G2" s="61"/>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="73" t="s">
+      <c r="I2" s="72" t="s">
         <v>72</v>
       </c>
       <c r="J2" s="61" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K2" s="61" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="61"/>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="72" t="s">
         <v>72</v>
       </c>
       <c r="D3" s="22" t="s">
@@ -7398,29 +7930,29 @@
       </c>
       <c r="G3" s="61"/>
       <c r="H3" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="I3" s="73" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="I3" s="74" t="s">
-        <v>237</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="75" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="77" t="s">
         <v>92</v>
       </c>
       <c r="E4" s="61"/>
@@ -7428,39 +7960,39 @@
       <c r="G4" s="8"/>
       <c r="H4" s="26"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="79"/>
+      <c r="J4" s="78"/>
       <c r="K4" s="26"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="77" t="s">
-        <v>232</v>
-      </c>
-      <c r="C5" s="80" t="s">
+      <c r="B5" s="76" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="74" t="s">
         <v>94</v>
       </c>
       <c r="E5" s="61"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="78"/>
-      <c r="J5" s="81"/>
+      <c r="H5" s="77"/>
+      <c r="J5" s="80"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="78" t="s">
+      <c r="D6" s="77" t="s">
         <v>97</v>
       </c>
       <c r="E6" s="61"/>
@@ -7469,200 +8001,200 @@
       <c r="J6" s="28"/>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="74" t="s">
         <v>100</v>
       </c>
       <c r="E7" s="61"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="74" t="s">
         <v>102</v>
       </c>
       <c r="E8" s="61"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="74" t="s">
         <v>52</v>
       </c>
       <c r="E9" s="61"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="81" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="82" t="s">
         <v>158</v>
       </c>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="82" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="74" t="s">
         <v>182</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="74" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="74" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="74" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="74" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="C15" s="75" t="s">
+      <c r="C15" s="74" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="74" t="s">
         <v>183</v>
       </c>
-      <c r="C16" s="77" t="s">
+      <c r="C16" s="76" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="74" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="74" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="74" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="81" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="74" t="s">
         <v>166</v>
       </c>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="74" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="74" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="82" t="s">
+      <c r="B24" s="81" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="83" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="75" t="s">
+      <c r="C25" s="74" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="75" t="s">
+      <c r="B26" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="75" t="s">
+      <c r="C26" s="74" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="75" t="s">
+      <c r="B27" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="C27" s="75" t="s">
+      <c r="C27" s="74" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="75" t="s">
+      <c r="B28" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="C28" s="75" t="s">
+      <c r="C28" s="74" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="75" t="s">
+      <c r="B29" s="74" t="s">
+        <v>205</v>
+      </c>
+      <c r="C29" s="82" t="s">
         <v>206</v>
       </c>
-      <c r="C29" s="83" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="82" t="s">
-        <v>212</v>
+      <c r="B30" s="81" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C31" s="61" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="61" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C32" s="61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -8316,7 +8848,7 @@
   <dimension ref="A2:K29"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8327,7 +8859,7 @@
     <col min="4" max="4" width="147.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="8.5703125"/>
     <col min="7" max="7" width="25.85546875"/>
-    <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
@@ -8355,7 +8887,7 @@
       <c r="E3" s="45"/>
       <c r="F3" s="22"/>
       <c r="G3" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
@@ -8366,14 +8898,14 @@
       <c r="A4" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="87" t="s">
-        <v>245</v>
-      </c>
-      <c r="D4" s="88" t="s">
+      <c r="C4" s="86" t="s">
         <v>244</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>243</v>
       </c>
       <c r="E4" s="45"/>
       <c r="F4" s="47"/>
@@ -8384,10 +8916,10 @@
       <c r="K4" s="48"/>
     </row>
     <row r="5" spans="1:11" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="89" t="s">
-        <v>246</v>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="88" t="s">
+        <v>245</v>
       </c>
       <c r="E5" s="45"/>
       <c r="F5" s="47"/>
@@ -8430,10 +8962,10 @@
         <v>113</v>
       </c>
       <c r="D8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G8" s="55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -8444,10 +8976,10 @@
         <v>115</v>
       </c>
       <c r="G9" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H9" s="63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -8458,10 +8990,10 @@
         <v>117</v>
       </c>
       <c r="G10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -8472,10 +9004,10 @@
         <v>119</v>
       </c>
       <c r="G11" t="s">
+        <v>199</v>
+      </c>
+      <c r="H11" t="s">
         <v>200</v>
-      </c>
-      <c r="H11" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -8486,10 +9018,10 @@
         <v>121</v>
       </c>
       <c r="G12" t="s">
+        <v>202</v>
+      </c>
+      <c r="H12" t="s">
         <v>203</v>
-      </c>
-      <c r="H12" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -8499,27 +9031,36 @@
       <c r="C13" t="s">
         <v>122</v>
       </c>
-      <c r="D13" s="86" t="s">
-        <v>243</v>
+      <c r="D13" s="85" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G14" s="90" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="84" t="s">
         <v>240</v>
       </c>
-      <c r="C14" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="85" t="s">
+      <c r="C15" t="s">
         <v>241</v>
       </c>
-      <c r="C15" t="s">
-        <v>242</v>
-      </c>
-      <c r="D15" s="89" t="s">
-        <v>247</v>
+      <c r="D15" s="88" t="s">
+        <v>246</v>
+      </c>
+      <c r="G15" s="89" t="s">
+        <v>251</v>
+      </c>
+      <c r="H15" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -8528,6 +9069,12 @@
       </c>
       <c r="C16" s="38" t="s">
         <v>124</v>
+      </c>
+      <c r="G16" s="89" t="s">
+        <v>253</v>
+      </c>
+      <c r="H16" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
clear + element positioning relative - father > absolute sons
</commit_message>
<xml_diff>
--- a/Omnifood/Documantation/omniFood.xlsx
+++ b/Omnifood/Documantation/omniFood.xlsx
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="286">
   <si>
     <t>Day</t>
   </si>
@@ -1782,38 +1782,6 @@
     <t>Make an element float in the assigned location</t>
   </si>
   <si>
-    <r>
-      <t>clear</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000CD"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t> both</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
     <t>Do not allow floating elements on the left or the right side of a specified element
 can be a &lt;div&gt; &lt;p&gt; …</t>
   </si>
@@ -1935,6 +1903,42 @@
   </si>
   <si>
     <t>CSS Selectors can select all / part of the selection</t>
+  </si>
+  <si>
+    <t>0300</t>
+  </si>
+  <si>
+    <r>
+      <t>clear</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> both</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>; inside a class
+https://css-tricks.com/snippets/css/clear-fix/</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2699,12 +2703,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2734,6 +2732,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2947,11 +2951,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="97117696"/>
-        <c:axId val="53768128"/>
+        <c:axId val="89773568"/>
+        <c:axId val="67137472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97117696"/>
+        <c:axId val="89773568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2989,7 +2993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53768128"/>
+        <c:crossAx val="67137472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2997,7 +3001,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53768128"/>
+        <c:axId val="67137472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3045,7 +3049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97117696"/>
+        <c:crossAx val="89773568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3210,7 +3214,7 @@
             <c:strRef>
               <c:f>'Duration Meter'!$C$3:$C$179</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>24/1/18</c:v>
                 </c:pt>
@@ -3219,6 +3223,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7/2/2018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11/2/2018</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3230,16 +3237,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="177"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3377,11 +3384,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53769856"/>
-        <c:axId val="53770432"/>
+        <c:axId val="67139200"/>
+        <c:axId val="67139776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53769856"/>
+        <c:axId val="67139200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3419,12 +3426,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53770432"/>
+        <c:crossAx val="67139776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53770432"/>
+        <c:axId val="67139776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3472,7 +3479,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53769856"/>
+        <c:crossAx val="67139200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4423,8 +4430,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>3352800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6441,7 +6448,7 @@
   <dimension ref="A1:AMK47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6525,11 +6532,11 @@
       </c>
       <c r="F3" s="11">
         <f>IFERROR(E3/$G$3,"-")</f>
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="G3" s="62">
         <f>SUM(E3:E81)</f>
-        <v>300</v>
+        <v>480</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="13"/>
@@ -6566,7 +6573,7 @@
       </c>
       <c r="F4" s="11">
         <f t="shared" ref="F4:F47" si="0">IFERROR(E4/$G$3,"-")</f>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>10</v>
@@ -6606,11 +6613,11 @@
       </c>
       <c r="F5" s="11">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="G5" s="61">
         <f>G3/60</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="13"/>
@@ -6632,13 +6639,22 @@
       <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="10"/>
+      <c r="B6" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="60">
+        <v>43406</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="E6" s="10">
+        <f>VALUE(LEFT(D6,2))*60+VALUE(RIGHT(D6,2))</f>
+        <v>180</v>
+      </c>
       <c r="F6" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -7579,8 +7595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7597,33 +7613,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="104" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
       <c r="G1" s="59" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G2" s="65" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="92" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="C3" s="95" t="s">
         <v>282</v>
+      </c>
+      <c r="C3" s="93" t="s">
+        <v>281</v>
       </c>
       <c r="D3" s="3"/>
       <c r="G3" s="66" t="s">
@@ -7637,10 +7653,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="103" t="s">
         <v>72</v>
       </c>
       <c r="D4" s="22"/>
@@ -7655,7 +7671,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="94" t="s">
         <v>221</v>
       </c>
       <c r="C5" s="70"/>
@@ -7694,28 +7710,28 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="94" t="s">
         <v>226</v>
       </c>
       <c r="C9" s="70"/>
-      <c r="D9" s="93" t="s">
-        <v>278</v>
-      </c>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
+      <c r="D9" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="70" t="s">
         <v>227</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>279</v>
-      </c>
-      <c r="D10" s="93" t="s">
-        <v>275</v>
-      </c>
-      <c r="E10" s="93"/>
-      <c r="F10" s="93"/>
+        <v>278</v>
+      </c>
+      <c r="D10" s="105" t="s">
+        <v>274</v>
+      </c>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="70" t="s">
@@ -7725,13 +7741,13 @@
         <v>228</v>
       </c>
       <c r="D11" s="91" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7740,40 +7756,40 @@
         <v>257</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="95" t="s">
         <v>258</v>
       </c>
-      <c r="B13" s="104" t="s">
+      <c r="B13" s="102" t="s">
         <v>260</v>
       </c>
       <c r="C13" s="70" t="s">
         <v>255</v>
       </c>
       <c r="D13" s="91" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="70" t="s">
         <v>259</v>
       </c>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="102" t="s">
         <v>261</v>
       </c>
       <c r="C14" s="70" t="s">
@@ -7796,36 +7812,36 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="98" t="s">
+    <row r="17" spans="2:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="B17" s="96" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" s="99" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B18" s="97" t="s">
+        <v>266</v>
+      </c>
+      <c r="C18" s="98" t="s">
         <v>265</v>
       </c>
-      <c r="C17" s="70" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B18" s="99" t="s">
+    </row>
+    <row r="19" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B19" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" s="70" t="s">
         <v>267</v>
       </c>
-      <c r="C18" s="100" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B19" s="101" t="s">
-        <v>269</v>
-      </c>
-      <c r="C19" s="70" t="s">
-        <v>268</v>
-      </c>
     </row>
     <row r="20" spans="2:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B20" s="102" t="s">
-        <v>281</v>
-      </c>
-      <c r="C20" s="103" t="s">
+      <c r="B20" s="100" t="s">
         <v>280</v>
+      </c>
+      <c r="C20" s="101" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
8/3/2018 responsive web design css
</commit_message>
<xml_diff>
--- a/Omnifood/Documantation/omniFood.xlsx
+++ b/Omnifood/Documantation/omniFood.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="2655" windowHeight="3240" tabRatio="826" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="2655" windowHeight="3240" tabRatio="826"/>
   </bookViews>
   <sheets>
     <sheet name="Duration Meter" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="309">
   <si>
     <t>Day</t>
   </si>
@@ -1787,41 +1787,6 @@
   </si>
   <si>
     <r>
-      <t>display</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000CD"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t> none</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>;
-display: inline;
-display: block;
-display: inline-block;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">The display property specifies the display behavior of an element.
 </t>
     </r>
@@ -1943,12 +1908,198 @@
   <si>
     <t>Basic Colors</t>
   </si>
+  <si>
+    <t>Decide the wieght (boldness) of the font</t>
+  </si>
+  <si>
+    <t>font-wieght: (100-900) , bold, lighter, bolder</t>
+  </si>
+  <si>
+    <t>29/2/2018</t>
+  </si>
+  <si>
+    <t>5/3/2018</t>
+  </si>
+  <si>
+    <t>ViewPort - The viewport is the user's visible 
+area of a web page.</t>
+  </si>
+  <si>
+    <t>Measurement units</t>
+  </si>
+  <si>
+    <t>height: 100vh;</t>
+  </si>
+  <si>
+    <t>vw - 1 unit reflects 1/100th the width of the viewport</t>
+  </si>
+  <si>
+    <t>vh - 1 unit reflects 1/100th the height of the viewport</t>
+  </si>
+  <si>
+    <t>height: 100vw;</t>
+  </si>
+  <si>
+    <t>Moving Objects</t>
+  </si>
+  <si>
+    <t>top:
+bottom:
+right:
+left:</t>
+  </si>
+  <si>
+    <t>Change the position of the box</t>
+  </si>
+  <si>
+    <t>transform: translate(-50%,-50%)</t>
+  </si>
+  <si>
+    <t>translate(x,y) coordinates</t>
+  </si>
+  <si>
+    <t>Gradiantly change the image colors
+To create a linear gradient you must define at least two color stops. 
+Color stops are the colors you want to render smooth transitions among. 
+You can also set a starting point and a direction (or an angle) along with the gradient effect.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">background: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>linear-gradient</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>direction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>color-stop1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>color-stop2, ...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>Manipulating Text</t>
+  </si>
+  <si>
+    <t>text-transform:</t>
+  </si>
+  <si>
+    <t>letter-spacing:</t>
+  </si>
+  <si>
+    <t>word-spacing:</t>
+  </si>
+  <si>
+    <r>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000CD"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> none</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;
+display: inline; (inline - columns )
+display: block; ( line breaks - rows )
+display: inline-block; (inline block - doesn’t line break + has padding and margin )</t>
+    </r>
+  </si>
+  <si>
+    <t>5/3/2019</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="55" x14ac:knownFonts="1">
+  <fonts count="57" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2331,8 +2482,22 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2411,8 +2576,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2461,13 +2638,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2742,6 +2928,20 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2869,6 +3069,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2912,13 +3113,15 @@
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>'Duration Meter'!$I$3:$I$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HTML CSS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2927,7 +3130,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2954,11 +3157,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="74796544"/>
-        <c:axId val="50638784"/>
+        <c:axId val="82245120"/>
+        <c:axId val="48918464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74796544"/>
+        <c:axId val="82245120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2996,7 +3199,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50638784"/>
+        <c:crossAx val="48918464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3004,7 +3207,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50638784"/>
+        <c:axId val="48918464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3052,7 +3255,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74796544"/>
+        <c:crossAx val="82245120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3067,6 +3270,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3138,6 +3342,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3210,6 +3415,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3217,7 +3423,7 @@
             <c:strRef>
               <c:f>'Duration Meter'!$C$3:$C$179</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>24/1/18</c:v>
                 </c:pt>
@@ -3230,6 +3436,15 @@
                 <c:pt idx="3">
                   <c:v>11/2/2018</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>29/2/2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5/3/2018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5/3/2019</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:xVal>
@@ -3240,25 +3455,25 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="177"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>0.14285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.125</c:v>
+                  <c:v>7.1428571428571425E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0.14285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.375</c:v>
+                  <c:v>0.21428571428571427</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.14285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.14285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.14285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3387,11 +3602,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50640512"/>
-        <c:axId val="50641088"/>
+        <c:axId val="48920192"/>
+        <c:axId val="48920768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50640512"/>
+        <c:axId val="48920192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3429,12 +3644,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50641088"/>
+        <c:crossAx val="48920768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50641088"/>
+        <c:axId val="48920768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3482,7 +3697,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50640512"/>
+        <c:crossAx val="48920192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4434,7 +4649,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>3352800</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4488,7 +4703,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1952625</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6505,8 +6720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6590,21 +6805,23 @@
       </c>
       <c r="F3" s="11">
         <f>IFERROR(E3/$G$3,"-")</f>
-        <v>0.25</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="G3" s="62">
         <f>SUM(E3:E81)</f>
-        <v>480</v>
+        <v>840</v>
       </c>
       <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
+      <c r="I3" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="J3" s="14">
         <f>COUNTIF($B$3:$B$500,I3)</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="15" t="e">
+        <v>7</v>
+      </c>
+      <c r="K3" s="15">
         <f>(J3/SUM($J$3:$J$7))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -6631,7 +6848,7 @@
       </c>
       <c r="F4" s="11">
         <f t="shared" ref="F4:F47" si="0">IFERROR(E4/$G$3,"-")</f>
-        <v>0.125</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>10</v>
@@ -6642,9 +6859,9 @@
         <f>COUNTIF($B$3:$B$500,I4)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="15" t="e">
+      <c r="K4" s="15">
         <f>(J4/SUM($J$3:$J$7))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -6671,11 +6888,11 @@
       </c>
       <c r="F5" s="11">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="G5" s="61">
         <f>G3/60</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="13"/>
@@ -6683,9 +6900,9 @@
         <f>COUNTIF($B$3:$B$500,I5)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="15" t="e">
+      <c r="K5" s="15">
         <f>(J5/SUM($J$3:$J$7))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -6704,7 +6921,7 @@
         <v>43406</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E6" s="10">
         <f>VALUE(LEFT(D6,2))*60+VALUE(RIGHT(D6,2))</f>
@@ -6712,7 +6929,7 @@
       </c>
       <c r="F6" s="11">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -6721,9 +6938,9 @@
         <f>COUNTIF($B$3:$B$500,I6)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="15" t="e">
+      <c r="K6" s="15">
         <f>(J6/SUM($J$3:$J$7))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -6735,13 +6952,22 @@
       <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="10"/>
+      <c r="B7" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" ref="E7:E9" si="1">VALUE(LEFT(D7,2))*60+VALUE(RIGHT(D7,2))</f>
+        <v>120</v>
+      </c>
       <c r="F7" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
@@ -6750,9 +6976,9 @@
         <f>COUNTIF($B$3:$B$500,I7)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="15" t="e">
+      <c r="K7" s="15">
         <f>(J7/SUM($J$3:$J$7))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -6764,13 +6990,22 @@
       <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="10"/>
+      <c r="B8" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
       <c r="F8" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
@@ -6787,13 +7022,22 @@
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="10"/>
+      <c r="B9" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
       <c r="F9" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="G9"/>
       <c r="H9"/>
@@ -7456,15 +7700,15 @@
       </c>
       <c r="L36" s="21">
         <f>SUM(F3:F38)</f>
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="M36" s="21">
         <f>L36^2</f>
-        <v>1</v>
+        <v>0.99999999999999956</v>
       </c>
       <c r="N36" s="17">
         <f>J36*L36</f>
-        <v>1035</v>
+        <v>1034.9999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
@@ -7506,7 +7750,7 @@
       </c>
       <c r="I38" s="3">
         <f>(I36*N36-J36*L36)/(I36*K36-(J36)^2)</f>
-        <v>-4.4681884409907724E-2</v>
+        <v>-4.4681884409907717E-2</v>
       </c>
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
@@ -7531,7 +7775,7 @@
       </c>
       <c r="I39" s="18">
         <f>((L36)*(K36)-(J36)*(N36)) / ((I36)*(K36)-(J36^2))</f>
-        <v>1.0499055636500998</v>
+        <v>1.0499055636500996</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
@@ -7651,17 +7895,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
@@ -7683,7 +7927,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G2" s="65" t="s">
         <v>213</v>
@@ -7694,10 +7938,10 @@
         <v>28</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C3" s="93" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D3" s="3"/>
       <c r="G3" s="66" t="s">
@@ -7773,7 +8017,7 @@
       </c>
       <c r="C9" s="70"/>
       <c r="D9" s="105" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E9" s="105"/>
       <c r="F9" s="105"/>
@@ -7783,10 +8027,10 @@
         <v>227</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D10" s="105" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E10" s="105"/>
       <c r="F10" s="105"/>
@@ -7799,13 +8043,13 @@
         <v>228</v>
       </c>
       <c r="D11" s="91" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7814,13 +8058,13 @@
         <v>257</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -7834,13 +8078,13 @@
         <v>255</v>
       </c>
       <c r="D13" s="91" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -7875,43 +8119,125 @@
         <v>264</v>
       </c>
       <c r="C17" s="99" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="D17" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="E17" s="106"/>
+      <c r="F17" s="106"/>
+    </row>
+    <row r="18" spans="2:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B18" s="97" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C18" s="98" t="s">
-        <v>265</v>
+        <v>307</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B19" s="99" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B20" s="100" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C20" s="101" t="s">
-        <v>279</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C21" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="108" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="109" t="s">
+        <v>294</v>
+      </c>
+      <c r="C23" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="109" t="s">
+        <v>293</v>
+      </c>
+      <c r="C24" t="s">
+        <v>295</v>
+      </c>
       <c r="G24" s="86" t="s">
-        <v>286</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="108" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>298</v>
+      </c>
+      <c r="C27" s="110" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="109" t="s">
+        <v>300</v>
+      </c>
+      <c r="C28" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B29" s="110" t="s">
+        <v>301</v>
+      </c>
+      <c r="C29" s="111" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="108" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="109" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="109" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="109" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>

</xml_diff>

<commit_message>
Section - using the grid.css - col span-1-of-4
</commit_message>
<xml_diff>
--- a/Omnifood/Documantation/omniFood.xlsx
+++ b/Omnifood/Documantation/omniFood.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="2655" windowHeight="3240" tabRatio="826" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="2655" windowHeight="3240" tabRatio="826"/>
   </bookViews>
   <sheets>
     <sheet name="Duration Meter" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="290">
   <si>
     <t>Day</t>
   </si>
@@ -1875,13 +1875,47 @@
     <t>HTML GLOBAL ATTRIBUTS ( class, id, data-*)</t>
   </si>
   <si>
-    <t>12/3/2020</t>
-  </si>
-  <si>
     <t>0430</t>
   </si>
   <si>
     <t>transition: param1 duration1,param2 …</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>The &lt;section&gt; tag defines sections in a document, such as chapters,
+ headers, footers, or any other sections of the document.</t>
+  </si>
+  <si>
+    <t>&lt;section&gt; &lt;/section&gt;</t>
+  </si>
+  <si>
+    <t>HTML Special commands</t>
+  </si>
+  <si>
+    <t>&amp;mdash;</t>
+  </si>
+  <si>
+    <t>"-" in the length of a capital M</t>
+  </si>
+  <si>
+    <t>The premium icon font for Ionic Framework.</t>
+  </si>
+  <si>
+    <t>ionicons</t>
+  </si>
+  <si>
+    <t>randomuser.me</t>
+  </si>
+  <si>
+    <t>A free, open-source API for generating random user data. Like Lorem Ipsum, but for people.</t>
+  </si>
+  <si>
+    <t>12/3/2019</t>
+  </si>
+  <si>
+    <t>11/3/2020</t>
   </si>
 </sst>
 </file>
@@ -2484,7 +2518,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2783,6 +2817,9 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2999,11 +3036,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="117822976"/>
-        <c:axId val="64253312"/>
+        <c:axId val="80205312"/>
+        <c:axId val="61173120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117822976"/>
+        <c:axId val="80205312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3041,7 +3078,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64253312"/>
+        <c:crossAx val="61173120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3049,7 +3086,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64253312"/>
+        <c:axId val="61173120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3097,7 +3134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117822976"/>
+        <c:crossAx val="80205312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3265,7 +3302,7 @@
             <c:strRef>
               <c:f>'Duration Meter'!$C$3:$C$179</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>24/1/18</c:v>
                 </c:pt>
@@ -3288,7 +3325,10 @@
                   <c:v>5/3/2019</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12/3/2020</c:v>
+                  <c:v>11/3/2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12/3/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3300,34 +3340,34 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="177"/>
                 <c:pt idx="0">
-                  <c:v>0.10810810810810811</c:v>
+                  <c:v>9.7560975609756101E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4054054054054057E-2</c:v>
+                  <c:v>4.878048780487805E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10810810810810811</c:v>
+                  <c:v>9.7560975609756101E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16216216216216217</c:v>
+                  <c:v>0.14634146341463414</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10810810810810811</c:v>
+                  <c:v>9.7560975609756101E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10810810810810811</c:v>
+                  <c:v>9.7560975609756101E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10810810810810811</c:v>
+                  <c:v>9.7560975609756101E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.24324324324324326</c:v>
+                  <c:v>0.21951219512195122</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>9.7560975609756101E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -3447,11 +3487,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64255040"/>
-        <c:axId val="64255616"/>
+        <c:axId val="61174848"/>
+        <c:axId val="61175424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64255040"/>
+        <c:axId val="61174848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3489,12 +3529,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64255616"/>
+        <c:crossAx val="61175424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64255616"/>
+        <c:axId val="61175424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3542,7 +3582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64255040"/>
+        <c:crossAx val="61174848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4607,7 +4647,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>461960</xdr:colOff>
+      <xdr:colOff>131760</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>354100</xdr:rowOff>
     </xdr:to>
@@ -4655,7 +4695,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>461960</xdr:colOff>
+      <xdr:colOff>131760</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>354100</xdr:rowOff>
     </xdr:to>
@@ -4704,8 +4744,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1989960</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>164320</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177020</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4752,8 +4792,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1989960</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>164320</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177020</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4800,8 +4840,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1989960</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>164320</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177020</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4848,8 +4888,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1971240</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>164680</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177380</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4899,8 +4939,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1971240</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>164680</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177380</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4950,8 +4990,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1971240</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>164680</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177380</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5605,8 +5645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5690,11 +5730,11 @@
       </c>
       <c r="F3" s="11">
         <f>IFERROR(E3/$G$3,"-")</f>
-        <v>0.10810810810810811</v>
+        <v>9.7560975609756101E-2</v>
       </c>
       <c r="G3" s="42">
         <f>SUM(E3:E81)</f>
-        <v>1110</v>
+        <v>1230</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="13" t="s">
@@ -5702,7 +5742,7 @@
       </c>
       <c r="J3" s="14">
         <f>COUNTIF($B$3:$B$500,I3)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K3" s="15">
         <f>(J3/SUM($J$3:$J$7))</f>
@@ -5733,7 +5773,7 @@
       </c>
       <c r="F4" s="11">
         <f t="shared" ref="F4:F10" si="0">IFERROR(E4/$G$3,"-")</f>
-        <v>5.4054054054054057E-2</v>
+        <v>4.878048780487805E-2</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>10</v>
@@ -5773,11 +5813,11 @@
       </c>
       <c r="F5" s="11">
         <f t="shared" si="0"/>
-        <v>0.10810810810810811</v>
+        <v>9.7560975609756101E-2</v>
       </c>
       <c r="G5" s="41">
         <f>G3/60</f>
-        <v>18.5</v>
+        <v>20.5</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="13"/>
@@ -5814,7 +5854,7 @@
       </c>
       <c r="F6" s="11">
         <f t="shared" si="0"/>
-        <v>0.16216216216216217</v>
+        <v>0.14634146341463414</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -5852,7 +5892,7 @@
       </c>
       <c r="F7" s="11">
         <f t="shared" si="0"/>
-        <v>0.10810810810810811</v>
+        <v>9.7560975609756101E-2</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
@@ -5905,7 +5945,7 @@
       </c>
       <c r="F9" s="11">
         <f t="shared" si="0"/>
-        <v>0.10810810810810811</v>
+        <v>9.7560975609756101E-2</v>
       </c>
       <c r="G9"/>
       <c r="H9"/>
@@ -5936,8 +5976,8 @@
         <v>120</v>
       </c>
       <c r="F10" s="11">
-        <f t="shared" si="0"/>
-        <v>0.10810810810810811</v>
+        <f>IFERROR(E12/$G$3,"-")</f>
+        <v>9.7560975609756101E-2</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -5958,10 +5998,10 @@
         <v>134</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>276</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>277</v>
       </c>
       <c r="E11" s="10">
         <f t="shared" ref="E11" si="2">VALUE(LEFT(D11,2))*60+VALUE(RIGHT(D11,2))</f>
@@ -5969,7 +6009,7 @@
       </c>
       <c r="F11" s="11">
         <f>IFERROR(E11/$G$3,"-")</f>
-        <v>0.24324324324324326</v>
+        <v>0.21951219512195122</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
@@ -5986,13 +6026,22 @@
       <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="10"/>
+      <c r="B12" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="10">
+        <f>VALUE(LEFT(D12,2))*60+VALUE(RIGHT(D12,2))</f>
+        <v>120</v>
+      </c>
       <c r="F12" s="11">
         <f t="shared" ref="F12:F47" si="3">IFERROR(E12/$G$3,"-")</f>
-        <v>0</v>
+        <v>9.7560975609756101E-2</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -6586,15 +6635,15 @@
       </c>
       <c r="L36" s="20">
         <f>SUM(F3:F38)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="M36" s="20">
         <f>L36^2</f>
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="N36" s="16">
         <f>J36*L36</f>
-        <v>1035</v>
+        <v>1034.9999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
@@ -6636,7 +6685,7 @@
       </c>
       <c r="I38" s="3">
         <f>(I36*N36-J36*L36)/(I36*K36-(J36)^2)</f>
-        <v>-4.4681884409907724E-2</v>
+        <v>-4.4681884409907717E-2</v>
       </c>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
@@ -6661,7 +6710,7 @@
       </c>
       <c r="I39" s="17">
         <f>((L36)*(K36)-(J36)*(N36)) / ((I36)*(K36)-(J36^2))</f>
-        <v>1.0499055636500998</v>
+        <v>1.0499055636500996</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
@@ -6824,8 +6873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7230,7 +7279,7 @@
         <v>263</v>
       </c>
       <c r="C45" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -7272,10 +7321,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK33"/>
+  <dimension ref="A1:AMK36"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7287,7 +7336,7 @@
     <col min="5" max="5" width="18.5703125" style="54" customWidth="1"/>
     <col min="6" max="6" width="24.140625" style="54" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" style="54"/>
-    <col min="8" max="8" width="23" style="54"/>
+    <col min="8" max="8" width="28" style="54" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.5703125" style="54" customWidth="1"/>
     <col min="10" max="10" width="64" style="54"/>
     <col min="11" max="11" width="17.7109375" style="54"/>
@@ -7423,7 +7472,9 @@
       </c>
       <c r="E6" s="41"/>
       <c r="F6" s="22"/>
-      <c r="H6" s="23"/>
+      <c r="H6" s="51" t="s">
+        <v>281</v>
+      </c>
       <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7440,6 +7491,12 @@
         <v>42</v>
       </c>
       <c r="E7" s="41"/>
+      <c r="H7" s="54" t="s">
+        <v>283</v>
+      </c>
+      <c r="I7" s="54" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
@@ -7642,6 +7699,19 @@
       </c>
       <c r="C33" s="41" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="61" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="B36" s="119" t="s">
+        <v>279</v>
+      </c>
+      <c r="C36" s="54" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -7669,16 +7739,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -7714,10 +7784,35 @@
         <v>79</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" s="92" t="s">
+        <v>284</v>
+      </c>
+      <c r="C5" s="92" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C6" s="92" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4" display="http://ionicframework.com/"/>
+    <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
features section part 2 - icons / multiple classes element
</commit_message>
<xml_diff>
--- a/Omnifood/Documantation/omniFood.xlsx
+++ b/Omnifood/Documantation/omniFood.xlsx
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="295">
   <si>
     <t>Day</t>
   </si>
@@ -1916,6 +1916,21 @@
   </si>
   <si>
     <t>11/3/2020</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;</t>
+  </si>
+  <si>
+    <t>A range of text that is different from the normal text - technical terms, foreign language phrases, or fictional character thoughts. It is typically displayed in italic type.</t>
+  </si>
+  <si>
+    <t>.class:after</t>
+  </si>
+  <si>
+    <t>design right after the element</t>
+  </si>
+  <si>
+    <t>12/3/2020</t>
   </si>
 </sst>
 </file>
@@ -2779,6 +2794,9 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2817,9 +2835,6 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3036,11 +3051,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="80205312"/>
-        <c:axId val="61173120"/>
+        <c:axId val="115410432"/>
+        <c:axId val="115346816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80205312"/>
+        <c:axId val="115410432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3078,7 +3093,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61173120"/>
+        <c:crossAx val="115346816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3086,7 +3101,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61173120"/>
+        <c:axId val="115346816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3134,7 +3149,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80205312"/>
+        <c:crossAx val="115410432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3318,17 +3333,20 @@
                 <c:pt idx="4">
                   <c:v>29/2/2018</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="5">
                   <c:v>5/3/2018</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="6">
                   <c:v>5/3/2019</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="7">
                   <c:v>11/3/2020</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>12/3/2019</c:v>
+                </c:pt>
                 <c:pt idx="9">
-                  <c:v>12/3/2019</c:v>
+                  <c:v>12/3/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3340,34 +3358,34 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="177"/>
                 <c:pt idx="0">
-                  <c:v>9.7560975609756101E-2</c:v>
+                  <c:v>8.8888888888888892E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.878048780487805E-2</c:v>
+                  <c:v>4.4444444444444446E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.7560975609756101E-2</c:v>
+                  <c:v>8.8888888888888892E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14634146341463414</c:v>
+                  <c:v>0.13333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.7560975609756101E-2</c:v>
+                  <c:v>8.8888888888888892E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8.8888888888888892E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.7560975609756101E-2</c:v>
+                  <c:v>8.8888888888888892E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.7560975609756101E-2</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.21951219512195122</c:v>
+                  <c:v>8.8888888888888892E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.7560975609756101E-2</c:v>
+                  <c:v>8.8888888888888892E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -3487,11 +3505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61174848"/>
-        <c:axId val="61175424"/>
+        <c:axId val="115348544"/>
+        <c:axId val="115349120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61174848"/>
+        <c:axId val="115348544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3529,12 +3547,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61175424"/>
+        <c:crossAx val="115349120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61175424"/>
+        <c:axId val="115349120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3582,7 +3600,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61174848"/>
+        <c:crossAx val="115348544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4646,8 +4664,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>131760</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1020760</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>354100</xdr:rowOff>
     </xdr:to>
@@ -4694,8 +4712,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>131760</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1020760</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>354100</xdr:rowOff>
     </xdr:to>
@@ -4742,8 +4760,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1989960</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7628760</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>177020</xdr:rowOff>
     </xdr:to>
@@ -4790,8 +4808,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1989960</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7628760</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>177020</xdr:rowOff>
     </xdr:to>
@@ -4838,8 +4856,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1989960</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7628760</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>177020</xdr:rowOff>
     </xdr:to>
@@ -4886,8 +4904,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1971240</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7610040</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>177380</xdr:rowOff>
     </xdr:to>
@@ -4937,8 +4955,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1971240</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7610040</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>177380</xdr:rowOff>
     </xdr:to>
@@ -4988,8 +5006,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1971240</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7610040</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>177380</xdr:rowOff>
     </xdr:to>
@@ -5646,7 +5664,7 @@
   <dimension ref="A1:AMK47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5730,11 +5748,11 @@
       </c>
       <c r="F3" s="11">
         <f>IFERROR(E3/$G$3,"-")</f>
-        <v>9.7560975609756101E-2</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="G3" s="42">
         <f>SUM(E3:E81)</f>
-        <v>1230</v>
+        <v>1350</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="13" t="s">
@@ -5742,7 +5760,7 @@
       </c>
       <c r="J3" s="14">
         <f>COUNTIF($B$3:$B$500,I3)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K3" s="15">
         <f>(J3/SUM($J$3:$J$7))</f>
@@ -5772,8 +5790,8 @@
         <v>60</v>
       </c>
       <c r="F4" s="11">
-        <f t="shared" ref="F4:F10" si="0">IFERROR(E4/$G$3,"-")</f>
-        <v>4.878048780487805E-2</v>
+        <f t="shared" ref="F4:F9" si="0">IFERROR(E4/$G$3,"-")</f>
+        <v>4.4444444444444446E-2</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>10</v>
@@ -5813,11 +5831,11 @@
       </c>
       <c r="F5" s="11">
         <f t="shared" si="0"/>
-        <v>9.7560975609756101E-2</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="G5" s="41">
         <f>G3/60</f>
-        <v>20.5</v>
+        <v>22.5</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="13"/>
@@ -5854,7 +5872,7 @@
       </c>
       <c r="F6" s="11">
         <f t="shared" si="0"/>
-        <v>0.14634146341463414</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -5892,7 +5910,7 @@
       </c>
       <c r="F7" s="11">
         <f t="shared" si="0"/>
-        <v>9.7560975609756101E-2</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
@@ -5915,9 +5933,22 @@
       <c r="A8" s="8">
         <v>6</v>
       </c>
+      <c r="B8" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="10">
+        <f>VALUE(LEFT(D8,2))*60+VALUE(RIGHT(D8,2))</f>
+        <v>120</v>
+      </c>
       <c r="F8" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IFERROR(E8/$G$3,"-")</f>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="G8"/>
       <c r="L8" s="3"/>
@@ -5934,7 +5965,7 @@
         <v>134</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>135</v>
@@ -5944,8 +5975,8 @@
         <v>120</v>
       </c>
       <c r="F9" s="11">
-        <f t="shared" si="0"/>
-        <v>9.7560975609756101E-2</v>
+        <f>IFERROR(E11/$G$3,"-")</f>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="G9"/>
       <c r="H9"/>
@@ -5966,18 +5997,18 @@
         <v>134</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>249</v>
+        <v>289</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>135</v>
+        <v>276</v>
       </c>
       <c r="E10" s="10">
-        <f>VALUE(LEFT(D10,2))*60+VALUE(RIGHT(D10,2))</f>
-        <v>120</v>
+        <f t="shared" ref="E10" si="2">VALUE(LEFT(D10,2))*60+VALUE(RIGHT(D10,2))</f>
+        <v>270</v>
       </c>
       <c r="F10" s="11">
-        <f>IFERROR(E12/$G$3,"-")</f>
-        <v>9.7560975609756101E-2</v>
+        <f>IFERROR(E10/$G$3,"-")</f>
+        <v>0.2</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -5998,18 +6029,18 @@
         <v>134</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>276</v>
+        <v>135</v>
       </c>
       <c r="E11" s="10">
-        <f t="shared" ref="E11" si="2">VALUE(LEFT(D11,2))*60+VALUE(RIGHT(D11,2))</f>
-        <v>270</v>
+        <f>VALUE(LEFT(D11,2))*60+VALUE(RIGHT(D11,2))</f>
+        <v>120</v>
       </c>
       <c r="F11" s="11">
         <f>IFERROR(E11/$G$3,"-")</f>
-        <v>0.21951219512195122</v>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
@@ -6030,7 +6061,7 @@
         <v>134</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>135</v>
@@ -6040,8 +6071,8 @@
         <v>120</v>
       </c>
       <c r="F12" s="11">
-        <f t="shared" ref="F12:F47" si="3">IFERROR(E12/$G$3,"-")</f>
-        <v>9.7560975609756101E-2</v>
+        <f>IFERROR(E12/$G$3,"-")</f>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -6058,12 +6089,8 @@
       <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="10"/>
       <c r="F13" s="11">
-        <f t="shared" si="3"/>
+        <f>IFERROR(E13/$G$3,"-")</f>
         <v>0</v>
       </c>
       <c r="G13" s="3"/>
@@ -6086,7 +6113,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F12:F47" si="3">IFERROR(E14/$G$3,"-")</f>
         <v>0</v>
       </c>
       <c r="G14" s="3"/>
@@ -6635,15 +6662,15 @@
       </c>
       <c r="L36" s="20">
         <f>SUM(F3:F38)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="M36" s="20">
         <f>L36^2</f>
-        <v>0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="N36" s="16">
         <f>J36*L36</f>
-        <v>1034.9999999999998</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
@@ -6685,7 +6712,7 @@
       </c>
       <c r="I38" s="3">
         <f>(I36*N36-J36*L36)/(I36*K36-(J36)^2)</f>
-        <v>-4.4681884409907717E-2</v>
+        <v>-4.4681884409907724E-2</v>
       </c>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
@@ -6710,7 +6737,7 @@
       </c>
       <c r="I39" s="17">
         <f>((L36)*(K36)-(J36)*(N36)) / ((I36)*(K36)-(J36^2))</f>
-        <v>1.0499055636500996</v>
+        <v>1.0499055636500998</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
@@ -6874,7 +6901,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6892,13 +6919,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
       <c r="H1" s="39" t="s">
         <v>154</v>
       </c>
@@ -7003,11 +7030,11 @@
       </c>
       <c r="C9" s="50"/>
       <c r="D9" s="97"/>
-      <c r="E9" s="107" t="s">
+      <c r="E9" s="108" t="s">
         <v>218</v>
       </c>
-      <c r="F9" s="107"/>
-      <c r="G9" s="107"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="108"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="50" t="s">
@@ -7017,11 +7044,11 @@
         <v>219</v>
       </c>
       <c r="D10" s="97"/>
-      <c r="E10" s="107" t="s">
+      <c r="E10" s="108" t="s">
         <v>215</v>
       </c>
-      <c r="F10" s="107"/>
-      <c r="G10" s="107"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="108"/>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="50" t="s">
@@ -7116,11 +7143,11 @@
         <v>226</v>
       </c>
       <c r="D17" s="99"/>
-      <c r="E17" s="108" t="s">
+      <c r="E17" s="109" t="s">
         <v>231</v>
       </c>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="110"/>
     </row>
     <row r="18" spans="2:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B18" s="77" t="s">
@@ -7273,6 +7300,14 @@
         <v>253</v>
       </c>
       <c r="D42" s="90"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>293</v>
+      </c>
+      <c r="C43" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="89" t="s">
@@ -7324,13 +7359,13 @@
   <dimension ref="A1:AMK36"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" style="54"/>
-    <col min="2" max="2" width="84.5703125" style="54" customWidth="1"/>
+    <col min="2" max="2" width="153.28515625" style="54" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.85546875" style="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="54"/>
     <col min="5" max="5" width="18.5703125" style="54" customWidth="1"/>
@@ -7536,11 +7571,11 @@
       <c r="C12" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="116" t="s">
+      <c r="D12" s="117" t="s">
         <v>275</v>
       </c>
-      <c r="E12" s="117"/>
-      <c r="F12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="54" t="s">
@@ -7549,11 +7584,11 @@
       <c r="C13" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="D13" s="110" t="s">
+      <c r="D13" s="111" t="s">
         <v>274</v>
       </c>
-      <c r="E13" s="111"/>
-      <c r="F13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="113"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="54" t="s">
@@ -7562,9 +7597,9 @@
       <c r="C14" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="113"/>
-      <c r="E14" s="114"/>
-      <c r="F14" s="115"/>
+      <c r="D14" s="114"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="116"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="54" t="s">
@@ -7606,6 +7641,14 @@
         <v>104</v>
       </c>
     </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="54" t="s">
+        <v>291</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>290</v>
+      </c>
+    </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="61" t="s">
         <v>110</v>
@@ -7707,7 +7750,7 @@
       </c>
     </row>
     <row r="36" spans="2:3" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="B36" s="119" t="s">
+      <c r="B36" s="106" t="s">
         <v>279</v>
       </c>
       <c r="C36" s="54" t="s">

</xml_diff>

<commit_message>
Sections part 2 - Images lists in rows
</commit_message>
<xml_diff>
--- a/Omnifood/Documantation/omniFood.xlsx
+++ b/Omnifood/Documantation/omniFood.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="2655" windowHeight="3240" tabRatio="826"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="2655" windowHeight="3240" tabRatio="826" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Duration Meter" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="298">
   <si>
     <t>Day</t>
   </si>
@@ -1931,6 +1931,15 @@
   </si>
   <si>
     <t>12/3/2020</t>
+  </si>
+  <si>
+    <t>Containers</t>
+  </si>
+  <si>
+    <t>The &lt;figure&gt; tag specifies self-contained content, like illustrations, diagrams, photos, code listings, etc.</t>
+  </si>
+  <si>
+    <t>&lt;figure&gt; &lt;/figure&gt;</t>
   </si>
 </sst>
 </file>
@@ -3051,11 +3060,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="115410432"/>
-        <c:axId val="115346816"/>
+        <c:axId val="108451328"/>
+        <c:axId val="79129984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115410432"/>
+        <c:axId val="108451328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3093,7 +3102,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115346816"/>
+        <c:crossAx val="79129984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3101,7 +3110,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115346816"/>
+        <c:axId val="79129984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3149,7 +3158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115410432"/>
+        <c:crossAx val="108451328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3505,11 +3514,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115348544"/>
-        <c:axId val="115349120"/>
+        <c:axId val="79131712"/>
+        <c:axId val="79132288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115348544"/>
+        <c:axId val="79131712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3547,12 +3556,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115349120"/>
+        <c:crossAx val="79132288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115349120"/>
+        <c:axId val="79132288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3600,7 +3609,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115348544"/>
+        <c:crossAx val="79131712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4666,8 +4675,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1020760</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>354100</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>163600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4714,8 +4723,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1020760</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>354100</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>163600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5059,7 +5068,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>7600950</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5102,7 +5111,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>7600950</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5145,7 +5154,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>7600950</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5663,8 +5672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5790,7 +5799,7 @@
         <v>60</v>
       </c>
       <c r="F4" s="11">
-        <f t="shared" ref="F4:F9" si="0">IFERROR(E4/$G$3,"-")</f>
+        <f t="shared" ref="F4:F7" si="0">IFERROR(E4/$G$3,"-")</f>
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="G4" s="7" t="s">
@@ -6113,7 +6122,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11">
-        <f t="shared" ref="F12:F47" si="3">IFERROR(E14/$G$3,"-")</f>
+        <f t="shared" ref="F14:F47" si="3">IFERROR(E14/$G$3,"-")</f>
         <v>0</v>
       </c>
       <c r="G14" s="3"/>
@@ -7356,10 +7365,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK36"/>
+  <dimension ref="A1:AMK40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7512,7 +7521,7 @@
       </c>
       <c r="J6" s="24"/>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>30</v>
       </c>
@@ -7670,91 +7679,104 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="61" t="s">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="61" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="63" t="s">
+    <row r="26" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C26" s="54" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="54" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" s="54" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="54" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C28" s="54" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="54" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C30" s="62" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="B30" s="105" t="s">
+    <row r="31" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B31" s="105" t="s">
         <v>272</v>
       </c>
-      <c r="C30" s="104" t="s">
+      <c r="C31" s="104" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="61" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="61" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="41" t="s">
-        <v>149</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C34" s="41" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="61" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="61" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="B36" s="106" t="s">
+    <row r="37" spans="2:3" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="B37" s="106" t="s">
         <v>279</v>
       </c>
-      <c r="C36" s="54" t="s">
+      <c r="C37" s="54" t="s">
         <v>280</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="54" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="89" t="s">
+        <v>296</v>
+      </c>
+      <c r="C40" s="54" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>